<commit_message>
updated metrics and added prompts.txt
</commit_message>
<xml_diff>
--- a/metrics_results.xlsx
+++ b/metrics_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milind/Desktop/valence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milin\Desktop\valence_milind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F2F599-B3A5-A34A-90D7-663590A0540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384D8E0B-BDF7-4BE8-A603-4D8960B24559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{A7EE15EE-C3AE-404C-A817-28655A2E872B}"/>
+    <workbookView xWindow="8" yWindow="8" windowWidth="19185" windowHeight="11265" xr2:uid="{A7EE15EE-C3AE-404C-A817-28655A2E872B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="148">
   <si>
     <t>CountVec and XGB and no tuning</t>
   </si>
@@ -108,13 +108,385 @@
   </si>
   <si>
     <t>rho:0.4588338403702893</t>
+  </si>
+  <si>
+    <t>UAR:0.2252032520325203</t>
+  </si>
+  <si>
+    <t>kappa:0.003416856492027276</t>
+  </si>
+  <si>
+    <t>rho:0.32936374549819925</t>
+  </si>
+  <si>
+    <t>UAR:0.11733615221987315</t>
+  </si>
+  <si>
+    <t>kappa:0.04947526236881572</t>
+  </si>
+  <si>
+    <t>rho:0.26338433843384346</t>
+  </si>
+  <si>
+    <t>100 Prompt 1 0 shot 3.5</t>
+  </si>
+  <si>
+    <t>UAR:0.16723044397463002</t>
+  </si>
+  <si>
+    <t>kappa:0.022247413915261305</t>
+  </si>
+  <si>
+    <t>rho:0.1981038103810382</t>
+  </si>
+  <si>
+    <t>100 Prompt 3 0 shot short statistical input 3.5</t>
+  </si>
+  <si>
+    <t>100 Prompt 2 0 shot statistical input 3.5</t>
+  </si>
+  <si>
+    <t>100 Prompt 3 0 shot short statistical input 4-o-mini</t>
+  </si>
+  <si>
+    <t>UAR:0.19612403100775194</t>
+  </si>
+  <si>
+    <t>kappa:0.019529006318207864</t>
+  </si>
+  <si>
+    <t>rho:0.3489828982898291</t>
+  </si>
+  <si>
+    <t>UAR:0.19147286821705425</t>
+  </si>
+  <si>
+    <t>kappa:0.001777656228633906</t>
+  </si>
+  <si>
+    <t>rho:0.4154755475547556</t>
+  </si>
+  <si>
+    <t>100 Prompt 1 0 shot short statistical input 4-o-mini</t>
+  </si>
+  <si>
+    <t>100 Prompt 2 0 shot short statistical input 4-o-mini</t>
+  </si>
+  <si>
+    <t>UAR:0.06279069767441861</t>
+  </si>
+  <si>
+    <t>kappa:0.008705264612408392</t>
+  </si>
+  <si>
+    <t>rho:0.43632763276327635</t>
+  </si>
+  <si>
+    <t>UAR:0.1069767441860465</t>
+  </si>
+  <si>
+    <t>kappa:0.02857142857142847</t>
+  </si>
+  <si>
+    <t>rho:0.404992499249925</t>
+  </si>
+  <si>
+    <t>100 Prompt 1 1 shot 3.5</t>
+  </si>
+  <si>
+    <t>UAR:0.2735729386892177</t>
+  </si>
+  <si>
+    <t>kappa:0.028648715111275203</t>
+  </si>
+  <si>
+    <t>rho:0.46618661866186617</t>
+  </si>
+  <si>
+    <t>100 Prompt 2 1 shot 3.5</t>
+  </si>
+  <si>
+    <t>UAR:0.17829457364341086</t>
+  </si>
+  <si>
+    <t>kappa:0.01030110935023787</t>
+  </si>
+  <si>
+    <t>rho:0.24237023702370242</t>
+  </si>
+  <si>
+    <t>100 Prompt 3 1 shot 3.5</t>
+  </si>
+  <si>
+    <t>100 Prompt 3 1 shot 4-0-mini</t>
+  </si>
+  <si>
+    <t>kappa:0.025713081354503453</t>
+  </si>
+  <si>
+    <t>rho:0.4280828082808281</t>
+  </si>
+  <si>
+    <t>UAR:0.18449612403100774</t>
+  </si>
+  <si>
+    <t>kappa:0.009698419024843918</t>
+  </si>
+  <si>
+    <t>rho:0.4712571257125713</t>
+  </si>
+  <si>
+    <t>100 Prompt 2 1 shot 4-0-mini</t>
+  </si>
+  <si>
+    <t>UAR:0.20775193798449615</t>
+  </si>
+  <si>
+    <t>kappa:0.03762029746281714</t>
+  </si>
+  <si>
+    <t>rho:0.35106510651065115</t>
+  </si>
+  <si>
+    <t>100 Prompt 1 1 shot 4-0-mini</t>
+  </si>
+  <si>
+    <t>100 Prompt 1 3 shot 3.5</t>
+  </si>
+  <si>
+    <t>UAR:0.21388301620859762</t>
+  </si>
+  <si>
+    <t>kappa:0.0158311345646438</t>
+  </si>
+  <si>
+    <t>rho:0.3371677167716771</t>
+  </si>
+  <si>
+    <t>100 Prompt 2 3 shot 3.5</t>
+  </si>
+  <si>
+    <t>UAR:0.14947145877378437</t>
+  </si>
+  <si>
+    <t>kappa:0.04442970822281156</t>
+  </si>
+  <si>
+    <t>rho:0.10309030903090</t>
+  </si>
+  <si>
+    <t>UAR:0.15412262156448203</t>
+  </si>
+  <si>
+    <t>kappa:0.015481937739304286</t>
+  </si>
+  <si>
+    <t>rho:0.16037803780378046</t>
+  </si>
+  <si>
+    <t>100 Prompt 3 3 shot 3.5</t>
+  </si>
+  <si>
+    <t>UAR:0.1821705426356589</t>
+  </si>
+  <si>
+    <t>kappa:0.013958253297477352</t>
+  </si>
+  <si>
+    <t>rho:0.08868286828682859</t>
+  </si>
+  <si>
+    <t>100 Prompt 3 3 shot4-o-mini</t>
+  </si>
+  <si>
+    <t>UAR:0.20732910500352358</t>
+  </si>
+  <si>
+    <t>kappa:0.020408163265306145</t>
+  </si>
+  <si>
+    <t>rho:0.32208820882088207</t>
+  </si>
+  <si>
+    <t>100 Prompt 2 3 shot4-o-mini</t>
+  </si>
+  <si>
+    <t>UAR:0.2544749823819591</t>
+  </si>
+  <si>
+    <t>kappa:0.061473486625997276</t>
+  </si>
+  <si>
+    <t>rho:0.22544254425442545</t>
+  </si>
+  <si>
+    <t>100 Prompt 1 3 shot4-o-mini</t>
+  </si>
+  <si>
+    <t>3.5 &amp; 4omini performs poorer with more demonstration</t>
+  </si>
+  <si>
+    <t>UAR:0.10613107822410148</t>
+  </si>
+  <si>
+    <t>kappa:0.0167464114832534</t>
+  </si>
+  <si>
+    <t>rho:0.5521872187218722</t>
+  </si>
+  <si>
+    <t>100 Prompt 1 2 shot 3.5</t>
+  </si>
+  <si>
+    <t>UAR:0.15602536997885835</t>
+  </si>
+  <si>
+    <t>kappa:0.004648373069425782</t>
+  </si>
+  <si>
+    <t>rho:0.04420042004200431</t>
+  </si>
+  <si>
+    <t>100 Prompt 2 2 shot 3.5</t>
+  </si>
+  <si>
+    <t>100 Prompt 3 2 shot 3.5</t>
+  </si>
+  <si>
+    <t>UAR:0.1014799154334038</t>
+  </si>
+  <si>
+    <t>kappa:0.12794070254592338</t>
+  </si>
+  <si>
+    <t>rho:0.07179117911791177</t>
+  </si>
+  <si>
+    <t>UAR:0.08752642706131078</t>
+  </si>
+  <si>
+    <t>kappa:0.02758247701460248</t>
+  </si>
+  <si>
+    <t>rho:0.3787038703870387</t>
+  </si>
+  <si>
+    <t>100 Prompt 3 2 shot 4-0-mini</t>
+  </si>
+  <si>
+    <t>kappa:0.01036958255783027</t>
+  </si>
+  <si>
+    <t>rho:0.3037923792379238</t>
+  </si>
+  <si>
+    <t>100 Prompt 2 2 shot 4-0-mini</t>
+  </si>
+  <si>
+    <t>UAR:0.18682170542635657</t>
+  </si>
+  <si>
+    <t>kappa:0.027115858668857795</t>
+  </si>
+  <si>
+    <t>rho:0.31960396039603967</t>
+  </si>
+  <si>
+    <t>100 Prompt 1 2 shot 4-0-mini</t>
+  </si>
+  <si>
+    <t>kappa:0.0017424132423407013</t>
+  </si>
+  <si>
+    <t>rho:0.3421752727010908</t>
+  </si>
+  <si>
+    <t>500 Prompt 3 2 shot 4-0-mini unbiased dataset</t>
+  </si>
+  <si>
+    <t>500 Prompt 3 2 shot 3.5 unbiased dataset</t>
+  </si>
+  <si>
+    <t>kappa:0.013971522160572292</t>
+  </si>
+  <si>
+    <t>rho:0.22045883383533538</t>
+  </si>
+  <si>
+    <t>UAR:0.11380728554641598</t>
+  </si>
+  <si>
+    <t>UAR:0.09699818395470569</t>
+  </si>
+  <si>
+    <t>500 Prompt 1 2 shot 4-0-mini unbiased dataset</t>
+  </si>
+  <si>
+    <t>500 Prompt 1 2 shot 3.5 unbiased dataset</t>
+  </si>
+  <si>
+    <t>UAR:0.05207242815938469</t>
+  </si>
+  <si>
+    <t>kappa:0.01535666224573573</t>
+  </si>
+  <si>
+    <t>rho:0.44288073152292606</t>
+  </si>
+  <si>
+    <t>UAR:0.09723320158102768</t>
+  </si>
+  <si>
+    <t>kappa:0.01237753977785927</t>
+  </si>
+  <si>
+    <t>rho:0.20831857727430914</t>
+  </si>
+  <si>
+    <t>UAR:0.06974682192073496</t>
+  </si>
+  <si>
+    <t>kappa:0.0030883261272389717</t>
+  </si>
+  <si>
+    <t>rho:0.528656834627338</t>
+  </si>
+  <si>
+    <t>500 Prompt 1 3 shot 3.5 unbiased dataset</t>
+  </si>
+  <si>
+    <t>500 Prompt 1 3 shot mini4o unbiased dataset</t>
+  </si>
+  <si>
+    <t>UAR:0.0837731011644055</t>
+  </si>
+  <si>
+    <t>kappa:0.018100704996367734</t>
+  </si>
+  <si>
+    <t>rho:0.20676471505886018</t>
+  </si>
+  <si>
+    <t>UAR:0.042110885589146455</t>
+  </si>
+  <si>
+    <t>kappa:0.013324746905571283</t>
+  </si>
+  <si>
+    <t>rho:0.6054718778875116</t>
+  </si>
+  <si>
+    <t>500 Prompt 1 5 shot 35unbiased dataset</t>
+  </si>
+  <si>
+    <t>500 Prompt 1 5 shot mini4o unbiased dataset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,6 +499,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -150,9 +530,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,132 +868,760 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6F845C-7053-AC46-8816-9045B97E3D60}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A181" sqref="A181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A31" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A40" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A45" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A50" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A55" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A60" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A65" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A66" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A67" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A70" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A71" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A72" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A75" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A76" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A77" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A78" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A80" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A81" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A82" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A83" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A85" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A86" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A87" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A88" t="s">
+        <v>74</v>
+      </c>
+      <c r="G88" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A90" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A91" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A92" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A93" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A95" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A97" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A98" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A100" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A101" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A102" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A103" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A105" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A106" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A107" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A108" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A110" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A111" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A112" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A113" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A115" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A116" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A117" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A118" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A120" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A121" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A122" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A123" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A125" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A126" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A127" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A128" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A130" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A131" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A132" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A133" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A135" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A136" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A137" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A138" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A140" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A141" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A142" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A143" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A145" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A146" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A147" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A148" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A150" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A151" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A152" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A153" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A155" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A156" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A157" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A158" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A160" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A161" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A162" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A163" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A165" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A166" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A167" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A168" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A170" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A171" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A172" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A173" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A175" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A176" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A177" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A178" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A180" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented RAG and RAG Based LLM Prompting
</commit_message>
<xml_diff>
--- a/metrics_results.xlsx
+++ b/metrics_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milin\Desktop\valence_milind\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milind/Desktop/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384D8E0B-BDF7-4BE8-A603-4D8960B24559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E790FD2-6713-6B40-BF77-C8EF94F919F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8" yWindow="8" windowWidth="19185" windowHeight="11265" xr2:uid="{A7EE15EE-C3AE-404C-A817-28655A2E872B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19180" windowHeight="11260" xr2:uid="{A7EE15EE-C3AE-404C-A817-28655A2E872B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
   <si>
     <t>CountVec and XGB and no tuning</t>
   </si>
@@ -480,6 +480,78 @@
   </si>
   <si>
     <t>500 Prompt 1 5 shot mini4o unbiased dataset</t>
+  </si>
+  <si>
+    <t>UAR:0.0355897634563</t>
+  </si>
+  <si>
+    <t>kappa:0.03345673257</t>
+  </si>
+  <si>
+    <t>rho:0.55555555</t>
+  </si>
+  <si>
+    <t>UAR:0.1253498557846384</t>
+  </si>
+  <si>
+    <t>kappa:0.029007550654571057</t>
+  </si>
+  <si>
+    <t>rho:0.2436562226248905</t>
+  </si>
+  <si>
+    <t>coz it cannot generalzize</t>
+  </si>
+  <si>
+    <t>500 Prompt 1 3 shot 35unbiased dataset RAG</t>
+  </si>
+  <si>
+    <t>500 Prompt 1 3 shot mini4o unbiased dataset RAG</t>
+  </si>
+  <si>
+    <t>UAR:0.12395043264608482</t>
+  </si>
+  <si>
+    <t>kappa:0.014330110497237758</t>
+  </si>
+  <si>
+    <t>rho:0.23922114888459556</t>
+  </si>
+  <si>
+    <t>500 unbiased dataset RAG</t>
+  </si>
+  <si>
+    <t>UAR:0.599017199017199</t>
+  </si>
+  <si>
+    <t>kappa:0.9869308379946677</t>
+  </si>
+  <si>
+    <t>rho:0.9991096924387698</t>
+  </si>
+  <si>
+    <t>500 unbiased dataset RAG 3 extract</t>
+  </si>
+  <si>
+    <t>UAR:0.5956521739130435</t>
+  </si>
+  <si>
+    <t>kappa:0.9867120229616243</t>
+  </si>
+  <si>
+    <t>rho:0.9991442525770103</t>
+  </si>
+  <si>
+    <t>500 unbiased dataset RAG 2 extract</t>
+  </si>
+  <si>
+    <t>UAR:0.27362995406473667</t>
+  </si>
+  <si>
+    <t>kappa:0.46700507614213205</t>
+  </si>
+  <si>
+    <t>rho:0.9394815979263917</t>
   </si>
 </sst>
 </file>
@@ -868,390 +940,390 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6F845C-7053-AC46-8816-9045B97E3D60}">
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A181" sqref="A181"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="D209" sqref="D209"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>74</v>
       </c>
@@ -1259,369 +1331,487 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>152</v>
+      </c>
+      <c r="G187" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated folder structure; added test python files; plots added
</commit_message>
<xml_diff>
--- a/metrics_results.xlsx
+++ b/metrics_results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milind/Desktop/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E790FD2-6713-6B40-BF77-C8EF94F919F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC6EA3E-71AE-3240-A9FE-C7EB072AA5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19180" windowHeight="11260" xr2:uid="{A7EE15EE-C3AE-404C-A817-28655A2E872B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A7EE15EE-C3AE-404C-A817-28655A2E872B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,79 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
-  <si>
-    <t>CountVec and XGB and no tuning</t>
-  </si>
-  <si>
-    <t>UAR:0.20030539044886247</t>
-  </si>
-  <si>
-    <t>kappa:0.0010154953713358283</t>
-  </si>
-  <si>
-    <t>rho:0.39001736149072275</t>
-  </si>
-  <si>
-    <t>UAR:0.20013117442098793</t>
-  </si>
-  <si>
-    <t>kappa:0.0004547220323364298</t>
-  </si>
-  <si>
-    <t>rho:0.3964426672416208</t>
-  </si>
-  <si>
-    <t>TFIDF vec and XGB and no tuning</t>
-  </si>
-  <si>
-    <t>UAR:0.28061613881454556</t>
-  </si>
-  <si>
-    <t>kappa:0.039020692185513184</t>
-  </si>
-  <si>
-    <t>rho:0.4747612587302037</t>
-  </si>
-  <si>
-    <t>TFIDF vec and XGB and  finetuning</t>
-  </si>
-  <si>
-    <t>UAR:0.2870299741791537</t>
-  </si>
-  <si>
-    <t>kappa:0.07273671687806826</t>
-  </si>
-  <si>
-    <t>rho:0.49162915082445713</t>
-  </si>
-  <si>
-    <t>TFIDF vec and SVC and no finetuning</t>
-  </si>
-  <si>
-    <t>TFIDF vec and SVC and  finetuning</t>
-  </si>
-  <si>
-    <t>UAR:0.27832658569500673</t>
-  </si>
-  <si>
-    <t>kappa:0.027857401208080668</t>
-  </si>
-  <si>
-    <t>rho:0.4793906472872145</t>
-  </si>
-  <si>
-    <t>TFIDF vec and LR</t>
-  </si>
-  <si>
-    <t>UAR:0.2015877987335739</t>
-  </si>
-  <si>
-    <t>kappa:0.007953593307057139</t>
-  </si>
-  <si>
-    <t>rho:0.4588338403702893</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="160">
   <si>
     <t>UAR:0.2252032520325203</t>
   </si>
@@ -500,9 +429,6 @@
     <t>rho:0.2436562226248905</t>
   </si>
   <si>
-    <t>coz it cannot generalzize</t>
-  </si>
-  <si>
     <t>500 Prompt 1 3 shot 35unbiased dataset RAG</t>
   </si>
   <si>
@@ -552,6 +478,45 @@
   </si>
   <si>
     <t>rho:0.9394815979263917</t>
+  </si>
+  <si>
+    <t>UAR:0.22461275504753764</t>
+  </si>
+  <si>
+    <t>kappa:0.18008784773060016</t>
+  </si>
+  <si>
+    <t>rho:0.8800091200364801</t>
+  </si>
+  <si>
+    <t>500 unbiased dataset RAG 4 extract</t>
+  </si>
+  <si>
+    <t>500 unbiased dataset RAG 5 extract</t>
+  </si>
+  <si>
+    <t>UAR:0.2881476337998077</t>
+  </si>
+  <si>
+    <t>kappa:0.5503372470647014</t>
+  </si>
+  <si>
+    <t>rho:0.9461604886419546</t>
+  </si>
+  <si>
+    <t>Expt_Name</t>
+  </si>
+  <si>
+    <t>UAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kappa </t>
+  </si>
+  <si>
+    <t>Spearman</t>
+  </si>
+  <si>
+    <t>because it cannot generalzize</t>
   </si>
 </sst>
 </file>
@@ -940,560 +905,561 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6F845C-7053-AC46-8816-9045B97E3D60}">
-  <dimension ref="A1:G208"/>
+  <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="D209" sqref="D209"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H161" sqref="H161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="68.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
+      <c r="A9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
+      <c r="A10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>54</v>
+      <c r="G63" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>74</v>
-      </c>
-      <c r="G88" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
@@ -1513,62 +1479,62 @@
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
@@ -1578,240 +1544,232 @@
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
+      <c r="G162" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="s">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="s">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A175" s="2" t="s">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A180" s="2" t="s">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A185" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>152</v>
-      </c>
-      <c r="G187" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A190" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A195" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A200" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A205" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>171</v>
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A822B9B-A861-6C42-9FD1-2337ED863D16}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>